<commit_message>
fixed menu input during gameplay
</commit_message>
<xml_diff>
--- a/Algorithms for functionality - GameJam.xlsx
+++ b/Algorithms for functionality - GameJam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohit\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UE4 Projects\GameJam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB00887-B497-41F0-9321-574FB0721BCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7085EF3A-798B-4D67-BF12-BB223CB663F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Feature</t>
   </si>
@@ -136,16 +136,13 @@
     <t>if true add 1 to minutes and reset seconds to 0</t>
   </si>
   <si>
-    <t>For Setup:</t>
+    <t>check if can move based on if any player's are currently in QTE</t>
   </si>
   <si>
-    <t>Register player to QTE() in Level BP</t>
+    <t>if true:</t>
   </si>
   <si>
-    <t>Resgister HUD to QTE() in Level BP</t>
-  </si>
-  <si>
-    <t>Register HUD and QTE to QTE_Success(), QTE_CompleteSuccess(), QTE_Failure() events</t>
+    <t>set canMove for relevant player entry in the map</t>
   </si>
 </sst>
 </file>
@@ -448,21 +445,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E1003"/>
+  <dimension ref="A1:D1007"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" customWidth="1"/>
+    <col min="4" max="4" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,33 +471,27 @@
       </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="3"/>
       <c r="C4" s="5"/>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -508,22 +499,16 @@
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -531,7 +516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -539,235 +524,244 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="D11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="D12" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>21</v>
+      <c r="C17" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="9" t="s">
-        <v>22</v>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>23</v>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="6" t="s">
+        <v>19</v>
       </c>
-      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
-      <c r="B21" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="B21" s="7"/>
       <c r="C21" s="6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
-      <c r="C22" s="6" t="s">
-        <v>25</v>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="6" t="s">
-        <v>26</v>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
       <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>27</v>
+      <c r="A25" s="7"/>
+      <c r="B25" s="3" t="s">
+        <v>24</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
+      <c r="C25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
-      <c r="B26" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="B26" s="7"/>
       <c r="C26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
-      <c r="C28" s="6" t="s">
-        <v>30</v>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
       <c r="B29" s="7"/>
-      <c r="C29" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
+      <c r="B30" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="C30" s="6" t="s">
-        <v>32</v>
+        <v>14</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
+      <c r="C31" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>33</v>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="6" t="s">
+        <v>30</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
-      <c r="B33" s="3" t="s">
-        <v>18</v>
+      <c r="B33" s="7"/>
+      <c r="C33" s="6" t="s">
+        <v>31</v>
       </c>
-      <c r="C33" s="8"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
-      <c r="C35" s="6" t="s">
-        <v>35</v>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>33</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
       <c r="B36" s="7"/>
-      <c r="C36" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="C36" s="8"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
+      <c r="B37" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
+      <c r="C38" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
+      <c r="C39" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
+      <c r="C40" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
@@ -5584,6 +5578,26 @@
       <c r="B1003" s="7"/>
       <c r="C1003" s="8"/>
     </row>
+    <row r="1004" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1004" s="7"/>
+      <c r="B1004" s="7"/>
+      <c r="C1004" s="8"/>
+    </row>
+    <row r="1005" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1005" s="7"/>
+      <c r="B1005" s="7"/>
+      <c r="C1005" s="8"/>
+    </row>
+    <row r="1006" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1006" s="7"/>
+      <c r="B1006" s="7"/>
+      <c r="C1006" s="8"/>
+    </row>
+    <row r="1007" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1007" s="7"/>
+      <c r="B1007" s="7"/>
+      <c r="C1007" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing timer, Added Leaderboard
</commit_message>
<xml_diff>
--- a/Algorithms for functionality - GameJam.xlsx
+++ b/Algorithms for functionality - GameJam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohit\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UE4 Projects\GameJam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB00887-B497-41F0-9321-574FB0721BCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7085EF3A-798B-4D67-BF12-BB223CB663F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Feature</t>
   </si>
@@ -136,16 +136,13 @@
     <t>if true add 1 to minutes and reset seconds to 0</t>
   </si>
   <si>
-    <t>For Setup:</t>
+    <t>check if can move based on if any player's are currently in QTE</t>
   </si>
   <si>
-    <t>Register player to QTE() in Level BP</t>
+    <t>if true:</t>
   </si>
   <si>
-    <t>Resgister HUD to QTE() in Level BP</t>
-  </si>
-  <si>
-    <t>Register HUD and QTE to QTE_Success(), QTE_CompleteSuccess(), QTE_Failure() events</t>
+    <t>set canMove for relevant player entry in the map</t>
   </si>
 </sst>
 </file>
@@ -448,21 +445,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E1003"/>
+  <dimension ref="A1:D1007"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" customWidth="1"/>
+    <col min="4" max="4" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,33 +471,27 @@
       </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="3"/>
       <c r="C4" s="5"/>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -508,22 +499,16 @@
       <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -531,7 +516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -539,235 +524,244 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="D11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="D12" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>21</v>
+      <c r="C17" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="9" t="s">
-        <v>22</v>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>23</v>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="6" t="s">
+        <v>19</v>
       </c>
-      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
-      <c r="B21" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="B21" s="7"/>
       <c r="C21" s="6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
-      <c r="C22" s="6" t="s">
-        <v>25</v>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="6" t="s">
-        <v>26</v>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
       <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>27</v>
+      <c r="A25" s="7"/>
+      <c r="B25" s="3" t="s">
+        <v>24</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
+      <c r="C25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
-      <c r="B26" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="B26" s="7"/>
       <c r="C26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
-      <c r="C28" s="6" t="s">
-        <v>30</v>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
       <c r="B29" s="7"/>
-      <c r="C29" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
+      <c r="B30" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="C30" s="6" t="s">
-        <v>32</v>
+        <v>14</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
+      <c r="C31" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>33</v>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="6" t="s">
+        <v>30</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
-      <c r="B33" s="3" t="s">
-        <v>18</v>
+      <c r="B33" s="7"/>
+      <c r="C33" s="6" t="s">
+        <v>31</v>
       </c>
-      <c r="C33" s="8"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
-      <c r="C35" s="6" t="s">
-        <v>35</v>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>33</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
       <c r="B36" s="7"/>
-      <c r="C36" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="C36" s="8"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
+      <c r="B37" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
+      <c r="C38" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
+      <c r="C39" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
+      <c r="C40" s="6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
@@ -5584,6 +5578,26 @@
       <c r="B1003" s="7"/>
       <c r="C1003" s="8"/>
     </row>
+    <row r="1004" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1004" s="7"/>
+      <c r="B1004" s="7"/>
+      <c r="C1004" s="8"/>
+    </row>
+    <row r="1005" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1005" s="7"/>
+      <c r="B1005" s="7"/>
+      <c r="C1005" s="8"/>
+    </row>
+    <row r="1006" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1006" s="7"/>
+      <c r="B1006" s="7"/>
+      <c r="C1006" s="8"/>
+    </row>
+    <row r="1007" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1007" s="7"/>
+      <c r="B1007" s="7"/>
+      <c r="C1007" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>